<commit_message>
Update to PerformanceReport and WorstQueriesByPlanId
</commit_message>
<xml_diff>
--- a/ExcelTemplates/PerformanceReport.xlsx
+++ b/ExcelTemplates/PerformanceReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Version Control\GitHub\SQLServerPerformanceTuning\ExcelTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Version Control\Github\SQLServerPerformanceTuning\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22010B19-1F07-4E80-8A84-E38093081792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D36A91-3EB4-442C-BF2D-DA98FDE0D77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="5" xr2:uid="{E57F5ADB-DFB2-48C1-AB7B-5552241A8B93}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{E57F5ADB-DFB2-48C1-AB7B-5552241A8B93}"/>
   </bookViews>
   <sheets>
     <sheet name="PerformanceCharts" sheetId="16" r:id="rId1"/>
@@ -466,51 +466,6 @@
   </cellStyles>
   <dxfs count="91">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -943,6 +898,51 @@
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -959,7 +959,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2009,7 +2009,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3059,7 +3059,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4079,7 +4079,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -9218,17 +9218,17 @@
     <tableColumn id="2" xr3:uid="{0C6C0BB7-79E5-4371-B212-3A4A2331DBDF}" name="End Time UTC"/>
     <tableColumn id="9" xr3:uid="{40B8BD5F-5040-4223-9346-0B2C918A4E52}" name="Day of Week"/>
     <tableColumn id="10" xr3:uid="{1564472E-A30D-4F24-827F-1F64A863B8A8}" name="Hour"/>
-    <tableColumn id="11" xr3:uid="{5284FA1A-0967-4E7E-BE5B-A7A5731C1702}" name="Day of Week Hour" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{5284FA1A-0967-4E7E-BE5B-A7A5731C1702}" name="Day of Week Hour" dataDxfId="90"/>
     <tableColumn id="3" xr3:uid="{8050A426-A19A-4233-8658-75BB8746C5AD}" name="Total Executions" totalsRowFunction="custom">
       <totalsRowFormula>SUM(Table15[Total Executions])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4D33CF1D-5CEC-416B-A9F5-6A1E8151856D}" name="Duration Minutes" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{7A43699E-2F36-451B-90A6-62FDA8C59059}" name="CPU Minutes" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{88A63FC3-9937-4998-89F4-FBCA12CE1442}" name="CPU %" totalsRowFunction="average" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{5B67EF55-F2B4-4168-A1A0-77E6EAC76324}" name="Logical Reads GB" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{BB959A9E-1AFF-4B6A-A340-40AE52A86C30}" name="Physical Reads GB" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{8BB5AB34-44FE-4611-83A4-9C38A5EEB9FB}" name="Logical Writes GB" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{120F13F6-3B27-4EC8-A5B2-6945531EFB9B}" name="Wait Time Minutes" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{4D33CF1D-5CEC-416B-A9F5-6A1E8151856D}" name="Duration Minutes" totalsRowFunction="sum" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{7A43699E-2F36-451B-90A6-62FDA8C59059}" name="CPU Minutes" totalsRowFunction="sum" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="6" xr3:uid="{88A63FC3-9937-4998-89F4-FBCA12CE1442}" name="CPU %" totalsRowFunction="average" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="7" xr3:uid="{5B67EF55-F2B4-4168-A1A0-77E6EAC76324}" name="Logical Reads GB" totalsRowFunction="sum" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="8" xr3:uid="{BB959A9E-1AFF-4B6A-A340-40AE52A86C30}" name="Physical Reads GB" totalsRowFunction="sum" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="12" xr3:uid="{8BB5AB34-44FE-4611-83A4-9C38A5EEB9FB}" name="Logical Writes GB" totalsRowFunction="sum" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="15" xr3:uid="{120F13F6-3B27-4EC8-A5B2-6945531EFB9B}" name="Wait Time Minutes" totalsRowFunction="sum" dataDxfId="77" totalsRowDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9241,9 +9241,9 @@
     <tableColumn id="1" xr3:uid="{A2E09763-A37E-4A05-A7E6-F7EF3586DD0D}" name="Database Name"/>
     <tableColumn id="2" xr3:uid="{8A3CF4DC-4DB9-460A-B38B-6DC12C0B5C74}" name="Query Id"/>
     <tableColumn id="3" xr3:uid="{BE59FBFD-89C6-4A52-999E-05926E3D2E95}" name="Object Name"/>
-    <tableColumn id="4" xr3:uid="{B38082DE-CF16-4E46-978A-941B4D81A322}" name="Execution Count" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{6BD3D9C5-46C9-40D2-B914-02FC89FCFEEF}" name="Average Rowcount" dataDxfId="65"/>
-    <tableColumn id="6" xr3:uid="{A6A99769-C597-47FB-B55C-2403E017ACF3}" name="Total Logical Writes GB" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{B38082DE-CF16-4E46-978A-941B4D81A322}" name="Execution Count" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{6BD3D9C5-46C9-40D2-B914-02FC89FCFEEF}" name="Average Rowcount" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{A6A99769-C597-47FB-B55C-2403E017ACF3}" name="Total Logical Writes GB" dataDxfId="49"/>
     <tableColumn id="7" xr3:uid="{256B31D9-AD72-4AA5-AC52-797797D5A734}" name="Writes %"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -9254,8 +9254,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E2C1FD56-78EF-425C-80FB-F8C6EF19DCA2}" name="Table479113" displayName="Table479113" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{F436E373-59BB-479B-8C56-67FFAE9AE7A0}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{12647B7E-9675-4A5A-8AE0-FFACB3E314A7}" name="Total Logical Writes GB" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{4CB88092-66E2-4DEB-87E0-5C4F55B3FF91}" name="Total Logical Writes TB" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{12647B7E-9675-4A5A-8AE0-FFACB3E314A7}" name="Total Logical Writes GB" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{4CB88092-66E2-4DEB-87E0-5C4F55B3FF91}" name="Total Logical Writes TB" dataDxfId="47"/>
     <tableColumn id="3" xr3:uid="{3FA79342-8BAD-4788-B27B-E64254166D90}" name="Total Query Count"/>
     <tableColumn id="4" xr3:uid="{DB044820-14C9-417A-A7A6-BE3BBDFBB8B4}" name="Total Query Count for 80% Writes"/>
   </tableColumns>
@@ -9268,16 +9268,16 @@
   <autoFilter ref="A4:K54" xr:uid="{07C6AC24-9F41-43A4-BF5C-141CD088317D}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{81F8B422-DF8E-4E60-85A4-CDE78D62D0E9}" name="Database Name"/>
-    <tableColumn id="2" xr3:uid="{0D906079-F3C8-4406-8E27-22E98D6FD8DB}" name="Query Id" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{2507F79C-E4F7-4C95-8FAB-4CC3CE9C5FFB}" name="Total Wait Minutes" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{7D83D941-33F0-41C9-8BBF-FE6C2C7EAB32}" name="Wait %" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{747338E7-A340-4E30-9091-E27AA68E26BD}" name="Parallelism Wait Minutes" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{4591956D-8774-4669-A9D0-3D2509AEC52C}" name="Network Wait Minutes" dataDxfId="57"/>
-    <tableColumn id="7" xr3:uid="{6C7CBFC0-BD97-4A02-85D4-C74F39BEC35C}" name="CPU Wait Minutes" dataDxfId="56"/>
-    <tableColumn id="8" xr3:uid="{F8F9B4A9-1B13-4503-9929-3D4C2B197FB4}" name="Unknown Wait Minutes" dataDxfId="55"/>
-    <tableColumn id="9" xr3:uid="{BC78ED5A-D844-42E4-971D-6DB99D773A51}" name="Disk Wait Minutes" dataDxfId="54"/>
-    <tableColumn id="10" xr3:uid="{0162BF70-263B-4E5D-8D33-4AB5308379D6}" name="Lock Wait Minutes" dataDxfId="53"/>
-    <tableColumn id="11" xr3:uid="{5C5A4B4F-3D7D-4784-89E7-111EC0C03988}" name="Buffer Latch Wait Minutes" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{0D906079-F3C8-4406-8E27-22E98D6FD8DB}" name="Query Id" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{2507F79C-E4F7-4C95-8FAB-4CC3CE9C5FFB}" name="Total Wait Minutes" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{7D83D941-33F0-41C9-8BBF-FE6C2C7EAB32}" name="Wait %" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{747338E7-A340-4E30-9091-E27AA68E26BD}" name="Parallelism Wait Minutes" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{4591956D-8774-4669-A9D0-3D2509AEC52C}" name="Network Wait Minutes" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{6C7CBFC0-BD97-4A02-85D4-C74F39BEC35C}" name="CPU Wait Minutes" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{F8F9B4A9-1B13-4503-9929-3D4C2B197FB4}" name="Unknown Wait Minutes" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{BC78ED5A-D844-42E4-971D-6DB99D773A51}" name="Disk Wait Minutes" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{0162BF70-263B-4E5D-8D33-4AB5308379D6}" name="Lock Wait Minutes" dataDxfId="38"/>
+    <tableColumn id="11" xr3:uid="{5C5A4B4F-3D7D-4784-89E7-111EC0C03988}" name="Buffer Latch Wait Minutes" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9287,8 +9287,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{54B5AFC2-4496-46D4-8E42-147F18AA2ECB}" name="Table422" displayName="Table422" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{1C5DB8F4-590E-4152-AFFB-249253798EE6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{53D48E9E-0F04-4026-BB87-89161E6671FA}" name="Total Wait Minutes" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{47F23455-4658-4D78-A3B4-0724B39E7136}" name="Total Duration Hours" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{53D48E9E-0F04-4026-BB87-89161E6671FA}" name="Total Wait Minutes" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{47F23455-4658-4D78-A3B4-0724B39E7136}" name="Total Duration Hours" dataDxfId="35"/>
     <tableColumn id="3" xr3:uid="{21153059-3537-435E-8B47-CC95059196E9}" name="Total Query Count"/>
     <tableColumn id="4" xr3:uid="{0D4E202C-221C-4732-BFDE-DF415B22C87A}" name="Total Query Count for 80% Duration"/>
   </tableColumns>
@@ -9297,18 +9297,18 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{710C7A2A-6352-458C-B146-506BAEACBE46}" name="Table11" displayName="Table11" ref="A1:I11" totalsRowShown="0" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{710C7A2A-6352-458C-B146-506BAEACBE46}" name="Table11" displayName="Table11" ref="A1:I11" totalsRowShown="0" dataDxfId="34">
   <autoFilter ref="A1:I11" xr:uid="{E51BD040-99F5-444D-8988-8F17973B4A32}"/>
   <tableColumns count="9">
-    <tableColumn id="7" xr3:uid="{68600BBE-CCAB-4330-A36A-8D38017F99B7}" name="Database Name" dataDxfId="48"/>
-    <tableColumn id="1" xr3:uid="{830DEAC2-BB1B-4454-917B-CF41FAF567A2}" name="Total Duration" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{9009EB12-913B-4812-8CB5-A6BBBB896997}" name="CPU" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{530840AE-18BB-411F-912E-1E03154D3181}" name="Logical Reads" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{5FCE6C21-F684-4A76-AC0B-7FA1543DEFA5}" name="Physical Reads" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{DDF7468C-9626-4B49-95CB-A37B72DBEA8B}" name="Logical Writes" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{ADD63B5C-A0A4-4712-BB81-7DE69CE65720}" name="Waits" dataDxfId="42"/>
-    <tableColumn id="9" xr3:uid="{7D839B69-6D13-40A6-A83A-71FE946D8365}" name="Overall" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{F0331B9F-0687-47ED-836A-7F8935F91862}" name="Query Statement Query" dataDxfId="40">
+    <tableColumn id="7" xr3:uid="{68600BBE-CCAB-4330-A36A-8D38017F99B7}" name="Database Name" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{830DEAC2-BB1B-4454-917B-CF41FAF567A2}" name="Total Duration" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{9009EB12-913B-4812-8CB5-A6BBBB896997}" name="CPU" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{530840AE-18BB-411F-912E-1E03154D3181}" name="Logical Reads" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{5FCE6C21-F684-4A76-AC0B-7FA1543DEFA5}" name="Physical Reads" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{DDF7468C-9626-4B49-95CB-A37B72DBEA8B}" name="Logical Writes" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{ADD63B5C-A0A4-4712-BB81-7DE69CE65720}" name="Waits" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{7D839B69-6D13-40A6-A83A-71FE946D8365}" name="Overall" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{F0331B9F-0687-47ED-836A-7F8935F91862}" name="Query Statement Query" dataDxfId="25">
       <calculatedColumnFormula>CONCATENATE("select database_name = N'", Table11[[#This Row],[Database Name]], "', q.query_id, t.query_sql_text from ", Table11[[#This Row],[Database Name]], ".sys.query_store_query q join  ", Table11[[#This Row],[Database Name]], ".sys.query_store_query_text t on t.query_text_id = q.query_text_id where q.query_id = ", Table11[[#This Row],[Overall]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9327,8 +9327,8 @@
     <tableColumn id="5" xr3:uid="{4C4B65D8-ACD0-4866-A366-6C9DDBDC7711}" name="Database Name"/>
     <tableColumn id="1" xr3:uid="{3BB94C17-1DF8-4460-905F-88C9F019E0DF}" name="Query Id"/>
     <tableColumn id="2" xr3:uid="{6C3C67E0-B7B2-4D0A-84A0-51D102BA1D3D}" name="Plan Id"/>
-    <tableColumn id="3" xr3:uid="{1829EC3B-2E68-4E87-B506-9BE3DAED7AA2}" name="Query Plan Query" dataDxfId="39">
-      <calculatedColumnFormula>CONCATENATE("select database_name = N'", Table12[[#This Row],[Database Name]], "', plan_id, cast(query_plan as xml) as query_plane from ", Table12[[#This Row],[Database Name]], ".sys.query_store_plan where plan_id = ", Table12[[#This Row],[Plan Id]])</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{1829EC3B-2E68-4E87-B506-9BE3DAED7AA2}" name="Query Plan Query" dataDxfId="24">
+      <calculatedColumnFormula>CONCATENATE("select database_name = N'", Table12[[#This Row],[Database Name]], "', plan_id, cast(query_plan as xml) as query_plan from ", Table12[[#This Row],[Database Name]], ".sys.query_store_plan where plan_id = ", Table12[[#This Row],[Plan Id]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -9336,42 +9336,42 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7670AAE7-476C-4ED1-BCF9-CF3EC7E34768}" name="Table13" displayName="Table13" ref="A1:P3" totalsRowCount="1" headerRowDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7670AAE7-476C-4ED1-BCF9-CF3EC7E34768}" name="Table13" displayName="Table13" ref="A1:P3" totalsRowCount="1" headerRowDxfId="23">
   <autoFilter ref="A1:P2" xr:uid="{BA2BC664-8FDD-4485-A867-25558324D9E2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:P2">
     <sortCondition ref="P2"/>
     <sortCondition ref="D2"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="17" xr3:uid="{BC04EF40-794A-476D-BEE5-3C16A645EAF3}" name="Database Name" dataDxfId="37"/>
-    <tableColumn id="1" xr3:uid="{6F27793A-6D96-4332-AF8F-E214B397B4F6}" name="Query Id" dataDxfId="36"/>
+    <tableColumn id="17" xr3:uid="{BC04EF40-794A-476D-BEE5-3C16A645EAF3}" name="Database Name" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{6F27793A-6D96-4332-AF8F-E214B397B4F6}" name="Query Id" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{5F7491E8-CC8E-4368-A40E-446D31A439F3}" name="Object Name"/>
     <tableColumn id="3" xr3:uid="{20EA2CD5-9AD0-4947-A761-88F21BB15DB2}" name="Plan Id"/>
     <tableColumn id="4" xr3:uid="{90343523-F827-4B71-9FFD-89EA58E217AD}" name="Execution Count"/>
-    <tableColumn id="5" xr3:uid="{3CAE4964-54EA-45F8-94F8-B0876F39FA5E}" name="Average Rowcount" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{8B88BF9C-91C2-4C2B-B9D7-EF02B0163898}" name="Avg DOP" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{EC8914FD-409B-4C00-853F-AAD8F09BFBE3}" name="Avg Memory Grant MB" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{778BF87D-30CB-4ED1-8957-95B635F027F5}" name="Total Duration Minutes" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="5" xr3:uid="{3CAE4964-54EA-45F8-94F8-B0876F39FA5E}" name="Average Rowcount" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{8B88BF9C-91C2-4C2B-B9D7-EF02B0163898}" name="Avg DOP" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{EC8914FD-409B-4C00-853F-AAD8F09BFBE3}" name="Avg Memory Grant MB" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{778BF87D-30CB-4ED1-8957-95B635F027F5}" name="Total Duration Minutes" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="13">
       <totalsRowFormula>SUM(Table13[Total Duration Minutes])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A9CF50FA-1B16-42B8-B627-BE7E5221D305}" name="Total CPU_x000a_Minutes" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="9" xr3:uid="{A9CF50FA-1B16-42B8-B627-BE7E5221D305}" name="Total CPU_x000a_Minutes" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="11">
       <totalsRowFormula>SUM(Table13[Total CPU
 Minutes])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0F8D4B6E-380C-4BE9-A80B-617917136E09}" name="Total Logical Reads GB" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="24">
+    <tableColumn id="10" xr3:uid="{0F8D4B6E-380C-4BE9-A80B-617917136E09}" name="Total Logical Reads GB" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="9">
       <totalsRowFormula>SUM(Table13[Total Logical Reads GB])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9A27FFF2-67DC-4BB4-B9FF-157529ACCC80}" name="Total Physical Reads GB" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="11" xr3:uid="{9A27FFF2-67DC-4BB4-B9FF-157529ACCC80}" name="Total Physical Reads GB" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="7">
       <totalsRowFormula>SUM(Table13[Total Physical Reads GB])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{D61BAAD1-B446-42BB-BFDF-5418C86C241A}" name="Total Logical Writes GB" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
+    <tableColumn id="12" xr3:uid="{D61BAAD1-B446-42BB-BFDF-5418C86C241A}" name="Total Logical Writes GB" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="5">
       <totalsRowFormula>SUM(Table13[Total Logical Writes GB])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{51DC44FB-7F87-4EBB-8F2B-08FE907D0F71}" name="Total Wait Minutes" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
+    <tableColumn id="16" xr3:uid="{51DC44FB-7F87-4EBB-8F2B-08FE907D0F71}" name="Total Wait Minutes" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="3">
       <totalsRowFormula>SUM(Table13[Total Wait Minutes])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{2C29A776-7BAF-4270-AF5C-05E32BA8316D}" name="Comment" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{1517B95F-9B30-4902-9B97-1ED61FC32C5F}" name="Order" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{2C29A776-7BAF-4270-AF5C-05E32BA8316D}" name="Comment" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{1517B95F-9B30-4902-9B97-1ED61FC32C5F}" name="Order" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9384,9 +9384,9 @@
     <tableColumn id="1" xr3:uid="{D99E3806-E955-48B1-BF80-94D0B9C5E488}" name="Database Name"/>
     <tableColumn id="2" xr3:uid="{0D347773-BF5F-400C-B298-9C2A567EB1DD}" name="Query Id"/>
     <tableColumn id="3" xr3:uid="{44B2700F-6949-4BE6-9B0B-E202E69EE586}" name="Object Name"/>
-    <tableColumn id="4" xr3:uid="{0134D41D-DE42-4446-8A83-D5E6F0A3C6F2}" name="Execution Count" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{DFB0CA1F-D0AA-48A7-A255-2F187DDD149F}" name="Average Rowcount" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{64A499F8-DC0E-4BED-AE4B-112BDC535BEA}" name="Total Duration Minutes" dataDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{0134D41D-DE42-4446-8A83-D5E6F0A3C6F2}" name="Execution Count" dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{DFB0CA1F-D0AA-48A7-A255-2F187DDD149F}" name="Average Rowcount" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{64A499F8-DC0E-4BED-AE4B-112BDC535BEA}" name="Total Duration Minutes" dataDxfId="73"/>
     <tableColumn id="7" xr3:uid="{F777716B-6A03-4F1F-AD6F-69B3F982756C}" name="Duration %"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -9397,8 +9397,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{851B528F-53F6-4B87-A197-27D491E4A5E5}" name="Table4" displayName="Table4" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{1C5DB8F4-590E-4152-AFFB-249253798EE6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9085365D-0419-4944-9C42-4A5C69372A37}" name="Total Duration Minutes" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{BD698495-EFD9-4DF5-A336-D0A554FC92E2}" name="Total Duration Hours" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{9085365D-0419-4944-9C42-4A5C69372A37}" name="Total Duration Minutes" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{BD698495-EFD9-4DF5-A336-D0A554FC92E2}" name="Total Duration Hours" dataDxfId="71"/>
     <tableColumn id="3" xr3:uid="{478FB05D-8669-4104-A260-F04657E8E680}" name="Total Query Count"/>
     <tableColumn id="4" xr3:uid="{C70577D5-269D-4DDC-9562-D8FA2C834368}" name="Total Query Count for 80% Duration"/>
   </tableColumns>
@@ -9413,11 +9413,11 @@
     <tableColumn id="1" xr3:uid="{C550E639-FE65-4C32-9877-CFBC3B1DDCEC}" name="Database Name"/>
     <tableColumn id="2" xr3:uid="{29903189-44C8-4C48-9E71-6CF5FCB00B47}" name="Query Id"/>
     <tableColumn id="3" xr3:uid="{8C6E9D5B-9A95-41C7-A0E7-736B10F3428D}" name="Object Name"/>
-    <tableColumn id="4" xr3:uid="{ADFB89E9-CFFE-4E58-8100-CCEAB11F8544}" name="Execution Count" dataDxfId="85"/>
-    <tableColumn id="5" xr3:uid="{81DAD776-5DB3-4A25-852F-EED2CC24E42B}" name="Average Rowcount" dataDxfId="84"/>
-    <tableColumn id="6" xr3:uid="{14AC14F1-0F62-4FBA-AC72-8E12114A0AF2}" name="Total CPU Minutes" dataDxfId="83"/>
-    <tableColumn id="7" xr3:uid="{9E785107-5CF2-4510-86F5-90DFA84BF9F5}" name="CPU %" dataDxfId="82"/>
-    <tableColumn id="8" xr3:uid="{76DAE894-86A8-4A84-83C8-7455C0C2F982}" name="Avergage DOP" dataDxfId="81"/>
+    <tableColumn id="4" xr3:uid="{ADFB89E9-CFFE-4E58-8100-CCEAB11F8544}" name="Execution Count" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{81DAD776-5DB3-4A25-852F-EED2CC24E42B}" name="Average Rowcount" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{14AC14F1-0F62-4FBA-AC72-8E12114A0AF2}" name="Total CPU Minutes" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{9E785107-5CF2-4510-86F5-90DFA84BF9F5}" name="CPU %" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{76DAE894-86A8-4A84-83C8-7455C0C2F982}" name="Avergage DOP" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9427,8 +9427,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{87EBB8D8-EA3F-4662-B513-72C13060BCA9}" name="Table47" displayName="Table47" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{53E70DB0-20A3-437E-9CAA-DEAB1FDE9451}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9095E4A0-439E-4F1A-8C88-F3992F90E83B}" name="Total CPU Minutes" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{4995BCE1-60BF-475E-B42C-B774DD00F6AA}" name="Average CPU %" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{9095E4A0-439E-4F1A-8C88-F3992F90E83B}" name="Total CPU Minutes" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{4995BCE1-60BF-475E-B42C-B774DD00F6AA}" name="Average CPU %" dataDxfId="64"/>
     <tableColumn id="3" xr3:uid="{DC89D818-8A3C-4E1A-A5E7-4805D919FAE4}" name="Total Query Count"/>
     <tableColumn id="4" xr3:uid="{84037834-E796-4020-91D1-8B80FDFE30BE}" name="Total Query Count for 80% CPU Hours"/>
   </tableColumns>
@@ -9443,11 +9443,11 @@
     <tableColumn id="1" xr3:uid="{61A1EF3A-B2C8-4C7B-9E40-6920760BA878}" name="Database Name"/>
     <tableColumn id="2" xr3:uid="{F85185DF-1097-4F98-9CA0-A65BA2BCBFCA}" name="Query Id"/>
     <tableColumn id="3" xr3:uid="{27798744-8B4E-4BF6-9AB3-4D82CA67541F}" name="Object Name"/>
-    <tableColumn id="4" xr3:uid="{E1786825-063B-4403-B2DB-B75475FC5EFD}" name="Execution Count" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{3A0CA7CB-33B2-41CD-B11F-AF4E24D61320}" name="Average Rowcount" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{2614F994-A461-4713-8F8D-6AAD1F962C3D}" name="Total Logical Reads GB" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{A0E5C7ED-1475-46C3-AA44-DE68801774CF}" name="Reads %" dataDxfId="75"/>
-    <tableColumn id="8" xr3:uid="{50189684-03D6-4CFE-992F-0ECC712DB852}" name="Avg Memory Grant MB" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{E1786825-063B-4403-B2DB-B75475FC5EFD}" name="Execution Count" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{3A0CA7CB-33B2-41CD-B11F-AF4E24D61320}" name="Average Rowcount" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{2614F994-A461-4713-8F8D-6AAD1F962C3D}" name="Total Logical Reads GB" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{A0E5C7ED-1475-46C3-AA44-DE68801774CF}" name="Reads %" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{50189684-03D6-4CFE-992F-0ECC712DB852}" name="Avg Memory Grant MB" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9457,8 +9457,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C087DD13-C4D2-4201-A260-EE30B6808105}" name="Table479" displayName="Table479" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{331E4F2E-A884-409C-BA32-394AE10D8B02}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2277ED77-39F7-4BD1-AF7A-E9FF6A655660}" name="Total Logical Reads GB" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{7A4B83BD-8261-4019-8F44-7FA319AC4CF0}" name="Total Logical Reads TB" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{2277ED77-39F7-4BD1-AF7A-E9FF6A655660}" name="Total Logical Reads GB" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{7A4B83BD-8261-4019-8F44-7FA319AC4CF0}" name="Total Logical Reads TB" dataDxfId="57"/>
     <tableColumn id="3" xr3:uid="{701747A8-D499-43E5-B98A-BCA57898E6A5}" name="Total Query Count"/>
     <tableColumn id="4" xr3:uid="{DEEBC34B-F26B-4B0F-9CC1-600B134C66A6}" name="Total Query Count for 80% Reads"/>
   </tableColumns>
@@ -9473,9 +9473,9 @@
     <tableColumn id="1" xr3:uid="{00A223D2-0ED2-403B-8F53-470F7AD28D20}" name="Database Name"/>
     <tableColumn id="2" xr3:uid="{A0FD67ED-86D3-484A-BAF2-3280123AF06E}" name="Query Id"/>
     <tableColumn id="3" xr3:uid="{9A28C61B-D2C6-49DA-BCD2-216052ECFB3A}" name="Object Name"/>
-    <tableColumn id="4" xr3:uid="{EB8B7E13-09C3-4D49-A3D1-73B608B08F31}" name="Execution Count" dataDxfId="71"/>
-    <tableColumn id="5" xr3:uid="{B1D50155-E7D2-42CE-88AE-7D7B08BA1EB7}" name="Average Rowcount" dataDxfId="70"/>
-    <tableColumn id="6" xr3:uid="{5AD41518-441E-49C0-8B18-DA9ECCB53812}" name="Total Physical Reads GB" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{EB8B7E13-09C3-4D49-A3D1-73B608B08F31}" name="Execution Count" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{B1D50155-E7D2-42CE-88AE-7D7B08BA1EB7}" name="Average Rowcount" dataDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{5AD41518-441E-49C0-8B18-DA9ECCB53812}" name="Total Physical Reads GB" dataDxfId="54"/>
     <tableColumn id="7" xr3:uid="{8A02A21C-6901-4DF1-95F4-73797BDF0457}" name="Reads %"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -9486,8 +9486,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F04D7D04-FF07-40A0-A60D-48580C8C793C}" name="Table47911" displayName="Table47911" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{6A801407-7862-49BC-8DA4-71F3CB6256A9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{01CA7D26-D49B-4F0C-8C8C-222DE394165A}" name="Total Physical Reads GB" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{9ACD8827-5BDF-472C-9D5A-ED333B6788AA}" name="Total Physical Reads TB" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{01CA7D26-D49B-4F0C-8C8C-222DE394165A}" name="Total Physical Reads GB" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{9ACD8827-5BDF-472C-9D5A-ED333B6788AA}" name="Total Physical Reads TB" dataDxfId="52"/>
     <tableColumn id="3" xr3:uid="{25D241D6-067D-4188-B2EA-548A1C78BEF1}" name="Total Query Count"/>
     <tableColumn id="4" xr3:uid="{EDD4249B-EFCA-4C76-8684-47877E4FEF76}" name="Total Query Count for 80% Reads"/>
   </tableColumns>
@@ -9798,7 +9798,7 @@
       <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9813,18 +9813,18 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.3984375" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -9838,11 +9838,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -9865,154 +9865,154 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
     </row>
   </sheetData>
@@ -10032,18 +10032,18 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.73046875" customWidth="1"/>
-    <col min="4" max="4" width="30.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -10057,11 +10057,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -10084,154 +10084,154 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
     </row>
   </sheetData>
@@ -10251,22 +10251,22 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -10280,10 +10280,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -10318,7 +10318,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
@@ -10328,7 +10328,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="F6" s="1"/>
@@ -10338,7 +10338,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
@@ -10348,7 +10348,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
@@ -10358,7 +10358,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
@@ -10368,7 +10368,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="F10" s="1"/>
@@ -10378,7 +10378,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
@@ -10388,7 +10388,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
@@ -10398,7 +10398,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
@@ -10408,7 +10408,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
@@ -10418,7 +10418,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
@@ -10428,7 +10428,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="F16" s="1"/>
@@ -10438,7 +10438,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
@@ -10448,7 +10448,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="F18" s="1"/>
@@ -10458,7 +10458,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
@@ -10468,7 +10468,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="F20" s="1"/>
@@ -10478,7 +10478,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="F21" s="1"/>
@@ -10488,7 +10488,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="F22" s="1"/>
@@ -10498,7 +10498,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="F23" s="1"/>
@@ -10508,7 +10508,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="F24" s="1"/>
@@ -10518,7 +10518,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="F25" s="1"/>
@@ -10528,7 +10528,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="F26" s="1"/>
@@ -10538,7 +10538,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="F27" s="1"/>
@@ -10548,7 +10548,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="F28" s="1"/>
@@ -10558,7 +10558,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="F29" s="1"/>
@@ -10568,7 +10568,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="F30" s="1"/>
@@ -10578,7 +10578,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="F31" s="1"/>
@@ -10588,7 +10588,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="F32" s="1"/>
@@ -10598,7 +10598,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="F33" s="1"/>
@@ -10608,7 +10608,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="F34" s="1"/>
@@ -10618,7 +10618,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="F35" s="1"/>
@@ -10628,7 +10628,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="F36" s="1"/>
@@ -10638,7 +10638,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="F37" s="1"/>
@@ -10648,7 +10648,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="F38" s="1"/>
@@ -10658,7 +10658,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="F39" s="1"/>
@@ -10668,7 +10668,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="F40" s="1"/>
@@ -10678,7 +10678,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="F41" s="1"/>
@@ -10688,7 +10688,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="F42" s="1"/>
@@ -10698,7 +10698,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="F43" s="1"/>
@@ -10708,7 +10708,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="F44" s="1"/>
@@ -10718,7 +10718,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="F45" s="1"/>
@@ -10728,7 +10728,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="F46" s="1"/>
@@ -10738,7 +10738,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="F47" s="1"/>
@@ -10748,7 +10748,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="F48" s="1"/>
@@ -10758,7 +10758,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="F49" s="1"/>
@@ -10768,7 +10768,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="F50" s="1"/>
@@ -10778,7 +10778,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="F51" s="1"/>
@@ -10788,7 +10788,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="F52" s="1"/>
@@ -10798,7 +10798,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="F53" s="1"/>
@@ -10808,7 +10808,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="F54" s="1"/>
@@ -10837,18 +10837,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.73046875" customWidth="1"/>
-    <col min="2" max="2" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1328125" customWidth="1"/>
-    <col min="4" max="5" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="16.73046875" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -10877,7 +10877,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -10891,7 +10891,7 @@
         <v xml:space="preserve">select database_name = N'', q.query_id, t.query_sql_text from .sys.query_store_query q join  .sys.query_store_query_text t on t.query_text_id = q.query_text_id where q.query_id = </v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -10905,7 +10905,7 @@
         <v xml:space="preserve">select database_name = N'', q.query_id, t.query_sql_text from .sys.query_store_query q join  .sys.query_store_query_text t on t.query_text_id = q.query_text_id where q.query_id = </v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="22"/>
@@ -10919,7 +10919,7 @@
         <v xml:space="preserve">select database_name = N'', q.query_id, t.query_sql_text from .sys.query_store_query q join  .sys.query_store_query_text t on t.query_text_id = q.query_text_id where q.query_id = </v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="22"/>
       <c r="C5" s="14"/>
@@ -10933,7 +10933,7 @@
         <v xml:space="preserve">select database_name = N'', q.query_id, t.query_sql_text from .sys.query_store_query q join  .sys.query_store_query_text t on t.query_text_id = q.query_text_id where q.query_id = </v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -10947,7 +10947,7 @@
         <v xml:space="preserve">select database_name = N'', q.query_id, t.query_sql_text from .sys.query_store_query q join  .sys.query_store_query_text t on t.query_text_id = q.query_text_id where q.query_id = </v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="22"/>
@@ -10961,7 +10961,7 @@
         <v xml:space="preserve">select database_name = N'', q.query_id, t.query_sql_text from .sys.query_store_query q join  .sys.query_store_query_text t on t.query_text_id = q.query_text_id where q.query_id = </v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -10975,7 +10975,7 @@
         <v xml:space="preserve">select database_name = N'', q.query_id, t.query_sql_text from .sys.query_store_query q join  .sys.query_store_query_text t on t.query_text_id = q.query_text_id where q.query_id = </v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -10989,7 +10989,7 @@
         <v xml:space="preserve">select database_name = N'', q.query_id, t.query_sql_text from .sys.query_store_query q join  .sys.query_store_query_text t on t.query_text_id = q.query_text_id where q.query_id = </v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -11003,7 +11003,7 @@
         <v xml:space="preserve">select database_name = N'', q.query_id, t.query_sql_text from .sys.query_store_query q join  .sys.query_store_query_text t on t.query_text_id = q.query_text_id where q.query_id = </v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -11014,7 +11014,7 @@
         <v xml:space="preserve">select database_name = N'', q.query_id, t.query_sql_text from .sys.query_store_query q join  .sys.query_store_query_text t on t.query_text_id = q.query_text_id where q.query_id = </v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -11023,7 +11023,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -11037,10 +11037,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" t="str">
-        <f>CONCATENATE("select database_name = N'", Table12[[#This Row],[Database Name]], "', plan_id, cast(query_plan as xml) as query_plane from ", Table12[[#This Row],[Database Name]], ".sys.query_store_plan where plan_id = ", Table12[[#This Row],[Plan Id]])</f>
-        <v xml:space="preserve">select database_name = N'', plan_id, cast(query_plan as xml) as query_plane from .sys.query_store_plan where plan_id = </v>
+        <f>CONCATENATE("select database_name = N'", Table12[[#This Row],[Database Name]], "', plan_id, cast(query_plan as xml) as query_plan from ", Table12[[#This Row],[Database Name]], ".sys.query_store_plan where plan_id = ", Table12[[#This Row],[Plan Id]])</f>
+        <v xml:space="preserve">select database_name = N'', plan_id, cast(query_plan as xml) as query_plan from .sys.query_store_plan where plan_id = </v>
       </c>
     </row>
   </sheetData>
@@ -11065,21 +11065,21 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.3984375" customWidth="1"/>
-    <col min="2" max="2" width="10.3984375" customWidth="1"/>
-    <col min="3" max="3" width="29.3984375" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.59765625" style="4" customWidth="1"/>
-    <col min="8" max="12" width="14.59765625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.5703125" style="4" customWidth="1"/>
+    <col min="8" max="12" width="14.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="1" customWidth="1"/>
     <col min="14" max="14" width="14" style="20" customWidth="1"/>
-    <col min="15" max="15" width="36.1328125" customWidth="1"/>
+    <col min="15" max="15" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
@@ -11129,13 +11129,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="14"/>
       <c r="N2" s="1"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I3" s="1">
         <f>SUM(Table13[Total Duration Minutes])</f>
         <v>0</v>
@@ -11163,7 +11163,7 @@
       </c>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>45</v>
       </c>
@@ -11212,17 +11212,17 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>59</v>
       </c>
@@ -11230,7 +11230,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>57</v>
       </c>
@@ -11241,12 +11241,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>58</v>
       </c>
@@ -11262,17 +11262,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>61</v>
       </c>
@@ -11280,7 +11280,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>57</v>
       </c>
@@ -11291,12 +11291,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>58</v>
       </c>
@@ -11312,17 +11312,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>62</v>
       </c>
@@ -11330,7 +11330,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>57</v>
       </c>
@@ -11341,12 +11341,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>58</v>
       </c>
@@ -11362,17 +11362,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>63</v>
       </c>
@@ -11380,7 +11380,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>57</v>
       </c>
@@ -11391,12 +11391,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>58</v>
       </c>
@@ -11414,26 +11414,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="31.1328125" customWidth="1"/>
-    <col min="5" max="5" width="31.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.59765625" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.46484375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31.1328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -11483,10 +11483,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -11541,18 +11541,18 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.59765625" customWidth="1"/>
-    <col min="4" max="4" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -11566,11 +11566,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -11593,154 +11593,154 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
     </row>
   </sheetData>
@@ -11761,19 +11761,19 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="42.73046875" customWidth="1"/>
-    <col min="4" max="4" width="33.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -11787,11 +11787,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -11817,252 +11817,252 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
       <c r="G5" s="1"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
       <c r="G6" s="1"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
       <c r="G7" s="1"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
       <c r="G8" s="1"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
       <c r="G9" s="1"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
       <c r="G10" s="1"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
       <c r="G11" s="1"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
       <c r="G12" s="1"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
       <c r="G13" s="1"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
       <c r="G14" s="1"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
       <c r="G15" s="1"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
       <c r="G16" s="1"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
       <c r="G17" s="1"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
       <c r="G18" s="1"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
       <c r="G19" s="1"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
       <c r="G20" s="1"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
       <c r="G21" s="1"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
       <c r="G22" s="1"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
       <c r="G24" s="1"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
       <c r="G25" s="1"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
       <c r="G26" s="1"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
       <c r="G27" s="1"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
       <c r="G28" s="1"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
       <c r="G29" s="1"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
       <c r="G30" s="1"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
       <c r="G31" s="1"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
       <c r="G32" s="1"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
       <c r="G33" s="1"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
       <c r="G34" s="1"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
       <c r="G35" s="1"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
       <c r="G36" s="1"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
       <c r="G37" s="1"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
       <c r="G38" s="1"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
       <c r="G39" s="1"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
       <c r="G40" s="1"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
       <c r="G41" s="1"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
       <c r="G42" s="1"/>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
       <c r="G43" s="1"/>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
       <c r="G44" s="1"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
       <c r="G45" s="1"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
       <c r="G46" s="1"/>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
       <c r="G47" s="1"/>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
       <c r="G48" s="1"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
       <c r="G49" s="1"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
       <c r="G50" s="1"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
       <c r="G51" s="1"/>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
       <c r="G52" s="1"/>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
       <c r="G53" s="1"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
       <c r="G54" s="1"/>
       <c r="H54" s="4"/>
@@ -12085,19 +12085,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.73046875" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -12111,11 +12111,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -12141,252 +12141,252 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="4:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>

</xml_diff>